<commit_message>
black out wrong numbers
</commit_message>
<xml_diff>
--- a/Simulation Sharpe Ratios.xlsx
+++ b/Simulation Sharpe Ratios.xlsx
@@ -47,7 +47,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -77,17 +77,37 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Mono;Courier New;Nimbus Mono L;DejaVu Sans Mono;Courier"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Liberation Mono;Courier New;Nimbus Mono L;DejaVu Sans Mono;Courier"/>
       <family val="3"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -124,7 +144,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -133,7 +153,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -161,12 +189,12 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,14 +247,14 @@
       <c r="C3" s="2" t="n">
         <v>0.1524048</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="3" t="n">
         <f aca="false">B3/C3</f>
         <v>1.15426745089394</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="4" t="n">
         <v>0.1890944</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="4" t="n">
         <v>0.1226764</v>
       </c>
       <c r="H3" s="1" t="n">
@@ -249,14 +277,14 @@
       <c r="C4" s="2" t="n">
         <v>0.1404221</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="3" t="n">
         <f aca="false">B4/C4</f>
         <v>1.24675959126092</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="4" t="n">
         <v>0.1922145</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="4" t="n">
         <v>0.1208315</v>
       </c>
       <c r="H4" s="1" t="n">
@@ -279,14 +307,14 @@
       <c r="C5" s="2" t="n">
         <v>0.1242882</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="3" t="n">
         <f aca="false">B5/C5</f>
         <v>1.37704786134162</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="4" t="n">
         <v>0.1921384</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="4" t="n">
         <v>0.119274</v>
       </c>
       <c r="H5" s="1" t="n">
@@ -309,14 +337,14 @@
       <c r="C6" s="2" t="n">
         <v>0.142538</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="3" t="n">
         <f aca="false">B6/C6</f>
         <v>1.18182028652009</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="4" t="n">
         <v>0.187696</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="4" t="n">
         <v>0.1208688</v>
       </c>
       <c r="H6" s="1" t="n">
@@ -339,14 +367,14 @@
       <c r="C7" s="2" t="n">
         <v>0.1325569</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="3" t="n">
         <f aca="false">B7/C7</f>
         <v>1.26517895334004</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="4" t="n">
         <v>0.1898371</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="4" t="n">
         <v>0.1192287</v>
       </c>
       <c r="H7" s="1" t="n">
@@ -368,14 +396,14 @@
       <c r="C8" s="2" t="n">
         <v>0.1192879</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="3" t="n">
         <f aca="false">B8/C8</f>
         <v>1.37682866409753</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="4" t="n">
         <v>0.1894266</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="4" t="n">
         <v>0.1179063</v>
       </c>
       <c r="H8" s="1" t="n">
@@ -398,14 +426,14 @@
       <c r="C9" s="2" t="n">
         <v>0.1332821</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="3" t="n">
         <f aca="false">B9/C9</f>
         <v>1.20790938918279</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="4" t="n">
         <v>0.1859094</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="4" t="n">
         <v>0.1190633</v>
       </c>
       <c r="H9" s="1" t="n">
@@ -428,14 +456,14 @@
       <c r="C10" s="2" t="n">
         <v>0.1252518</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="3" t="n">
         <f aca="false">B10/C10</f>
         <v>1.28017242067579</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="4" t="n">
         <v>0.1872086</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="4" t="n">
         <v>0.1176361</v>
       </c>
       <c r="H10" s="1" t="n">
@@ -458,14 +486,14 @@
       <c r="C11" s="2" t="n">
         <v>0.1147237</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="3" t="n">
         <f aca="false">B11/C11</f>
         <v>1.37135744401549</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="4" t="n">
         <v>0.1865636</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="4" t="n">
         <v>0.1165428</v>
       </c>
       <c r="H11" s="1" t="n">
@@ -478,24 +506,34 @@
         <v>0.229458736821077</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="F12" s="0"/>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0"/>
+      <c r="J12" s="0"/>
+    </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="5" t="n">
         <v>0.1617682</v>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="5" t="n">
         <v>0.1194213</v>
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">B13/C13</f>
         <v>1.35460089615504</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="4" t="n">
         <v>0.1890944</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="4" t="n">
         <v>0.1226764</v>
       </c>
       <c r="H13" s="1" t="n">
@@ -511,20 +549,20 @@
       <c r="A14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="5" t="n">
         <v>0.1615938</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="5" t="n">
         <v>0.1180623</v>
       </c>
       <c r="D14" s="1" t="n">
         <f aca="false">B14/C14</f>
         <v>1.36871634721668</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="4" t="n">
         <v>0.1922145</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="4" t="n">
         <v>0.1208315</v>
       </c>
       <c r="H14" s="1" t="n">
@@ -540,20 +578,20 @@
       <c r="A15" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="5" t="n">
         <v>0.1607831</v>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" s="5" t="n">
         <v>0.116948</v>
       </c>
       <c r="D15" s="1" t="n">
         <f aca="false">B15/C15</f>
         <v>1.37482556349831</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="4" t="n">
         <v>0.1921384</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="4" t="n">
         <v>0.119274</v>
       </c>
       <c r="H15" s="1" t="n">
@@ -569,20 +607,20 @@
       <c r="A16" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="5" t="n">
         <v>0.1600059</v>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" s="5" t="n">
         <v>0.1181483</v>
       </c>
       <c r="D16" s="1" t="n">
         <f aca="false">B16/C16</f>
         <v>1.35428017161483</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="4" t="n">
         <v>0.187696</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="4" t="n">
         <v>0.1208688</v>
       </c>
       <c r="H16" s="1" t="n">
@@ -598,20 +636,20 @@
       <c r="A17" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="5" t="n">
         <v>0.1598376</v>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" s="5" t="n">
         <v>0.1168691</v>
       </c>
       <c r="D17" s="1" t="n">
         <f aca="false">B17/C17</f>
         <v>1.36766347991043</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="4" t="n">
         <v>0.1898371</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="G17" s="4" t="n">
         <v>0.1192287</v>
       </c>
       <c r="H17" s="1" t="n">
@@ -627,20 +665,20 @@
       <c r="A18" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B18" s="3" t="n">
+      <c r="B18" s="5" t="n">
         <v>0.1590552</v>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" s="5" t="n">
         <v>0.1158209</v>
       </c>
       <c r="D18" s="1" t="n">
         <f aca="false">B18/C18</f>
         <v>1.37328582319771</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="4" t="n">
         <v>0.1894266</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="G18" s="4" t="n">
         <v>0.1179063</v>
       </c>
       <c r="H18" s="1" t="n">
@@ -656,20 +694,20 @@
       <c r="A19" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B19" s="3" t="n">
+      <c r="B19" s="5" t="n">
         <v>0.1582436</v>
       </c>
-      <c r="C19" s="3" t="n">
+      <c r="C19" s="5" t="n">
         <v>0.1169075</v>
       </c>
       <c r="D19" s="1" t="n">
         <f aca="false">B19/C19</f>
         <v>1.35357953937942</v>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="F19" s="4" t="n">
         <v>0.1859094</v>
       </c>
-      <c r="G19" s="2" t="n">
+      <c r="G19" s="4" t="n">
         <v>0.1190633</v>
       </c>
       <c r="H19" s="1" t="n">
@@ -685,20 +723,20 @@
       <c r="A20" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="5" t="n">
         <v>0.1580814</v>
       </c>
-      <c r="C20" s="3" t="n">
+      <c r="C20" s="5" t="n">
         <v>0.1157069</v>
       </c>
       <c r="D20" s="1" t="n">
         <f aca="false">B20/C20</f>
         <v>1.36622275767478</v>
       </c>
-      <c r="F20" s="2" t="n">
+      <c r="F20" s="4" t="n">
         <v>0.1872086</v>
       </c>
-      <c r="G20" s="2" t="n">
+      <c r="G20" s="4" t="n">
         <v>0.1176361</v>
       </c>
       <c r="H20" s="1" t="n">
@@ -714,20 +752,20 @@
       <c r="A21" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="5" t="n">
         <v>0.1573272</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="5" t="n">
         <v>0.1147237</v>
       </c>
       <c r="D21" s="1" t="n">
         <f aca="false">B21/C21</f>
         <v>1.37135744401549</v>
       </c>
-      <c r="F21" s="2" t="n">
+      <c r="F21" s="4" t="n">
         <v>0.1865636</v>
       </c>
-      <c r="G21" s="2" t="n">
+      <c r="G21" s="4" t="n">
         <v>0.1165428</v>
       </c>
       <c r="H21" s="1" t="n">

</xml_diff>